<commit_message>
demo added figs, uploaded figs, test rerun, update readme main
</commit_message>
<xml_diff>
--- a/Test/AUTO_inventory_template.xlsx
+++ b/Test/AUTO_inventory_template.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristakraskura/Github_repositories/Respirometry_Performances/Test/MANUAL/csv_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristakraskura/Github_repositories/AnalyzeResp_0/Test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A40F10-2E49-694C-BF18-751265451141}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E9070311-AE32-DC48-A0B9-BB70A95656AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940"/>
   </bookViews>
   <sheets>
-    <sheet name="MMR_inventory_template" sheetId="1" r:id="rId1"/>
+    <sheet name="SMR_inventory_template" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>date</t>
   </si>
@@ -31,23 +31,29 @@
     <t>channel</t>
   </si>
   <si>
-    <t>jul04</t>
+    <t>cycle_file_start</t>
   </si>
   <si>
-    <t>start</t>
+    <t>sectioned_slope_start</t>
   </si>
   <si>
-    <t>end</t>
+    <t>sectioned_slope_end</t>
   </si>
   <si>
-    <t>cycle</t>
+    <t>type</t>
+  </si>
+  <si>
+    <t>smr</t>
+  </si>
+  <si>
+    <t>jul04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -178,12 +184,6 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -530,9 +530,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -888,19 +887,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A3" sqref="A3:A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="5" max="12" width="16.6640625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -911,7 +907,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -919,52 +915,103 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B2">
         <v>4</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>10.9</v>
+        <v>489.5</v>
       </c>
       <c r="F2">
-        <v>13</v>
+        <v>494.5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B3">
         <v>4</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1134.5</v>
+      </c>
+      <c r="F3">
+        <v>1140</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4">
         <v>2</v>
       </c>
-      <c r="E3">
-        <v>10.3</v>
-      </c>
-      <c r="F3">
-        <v>14</v>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>38</v>
+      </c>
+      <c r="F4">
+        <v>42</v>
+      </c>
+      <c r="G4" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>23.16</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update, first full version
</commit_message>
<xml_diff>
--- a/Test/AUTO_inventory_template.xlsx
+++ b/Test/AUTO_inventory_template.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristakraskura/Github_repositories/AnalyzeResp_0/Test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E9070311-AE32-DC48-A0B9-BB70A95656AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBBE48E-B6CD-DC4D-8A3B-AEAD061284E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SMR_inventory_template" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>date</t>
   </si>
@@ -47,12 +47,48 @@
   </si>
   <si>
     <t>jul04</t>
+  </si>
+  <si>
+    <r>
+      <t>can write just default: 0 or write the start time if you want to discard the cycle</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>; this number is just the sanity check - it indicates what is the exact starting time of the cycle that will be "cleaned"</t>
+    </r>
+  </si>
+  <si>
+    <t>indicate the start time of the section to be KEPT, write 0 if you want to discard this cycle: in minutes</t>
+  </si>
+  <si>
+    <t>indicate the end time of the section to be KEPT, write 0 if you want to discard this cycle: in minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KEY </t>
+  </si>
+  <si>
+    <t>box number, must match with the original  filename</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date (three same as the file name). TIP: add ' symbol right before typing the date, because excel likes to change it in their date formats. </t>
+  </si>
+  <si>
+    <t>channel number, will be either 1,2,3,4; TIP: can read this off from the .png plot file while looking at what needs to be cleaned</t>
+  </si>
+  <si>
+    <t>for general cleaning - leave as is ('smr' for all). this comes in useful when slopes themselves are analysed, was used for Lobster anpnea (ask details if interested)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -189,7 +225,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -367,6 +403,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -530,9 +572,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -887,11 +931,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1011,6 +1055,67 @@
         <v>7</v>
       </c>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>